<commit_message>
added some external links to online resources
</commit_message>
<xml_diff>
--- a/researchFiles/API.xlsx
+++ b/researchFiles/API.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishna.sarma\personal\language-dependent-message-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishna.sarma\Desktop\Dissertation\researchFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3DAB2D-7436-43E1-A4B8-3C9D3589C1E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E6988C-57EB-480B-B3F2-F04B12317B51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" xr2:uid="{EBFCBB9B-FE7E-4A95-BB17-A77EE9FE8B3A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="266">
   <si>
     <t>Name</t>
   </si>
@@ -945,19 +945,21 @@
   <si>
     <t>1-500,000 free per month</t>
   </si>
+  <si>
+    <t>Git Hub links</t>
+  </si>
+  <si>
+    <t>https://github.com/googleapis/nodejs-translate/tree/master/samples</t>
+  </si>
+  <si>
+    <t>https://docs.aws.amazon.com/translate/latest/dg/examples-twitch.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1021,24 +1023,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1046,17 +1045,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1373,42 +1375,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0CC8E9-5E00-41C8-9AC3-477377C052F2}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+    <col min="4" max="4" width="67.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>262</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="13" t="s">
         <v>255</v>
       </c>
       <c r="D2" t="s">
@@ -1416,24 +1418,24 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="10"/>
+      <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="13"/>
       <c r="D3" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="10"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -1447,7 +1449,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
@@ -1455,32 +1457,32 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="255">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:4" ht="210">
+      <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="10" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B10">
@@ -1494,11 +1496,22 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="105">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="9" t="s">
         <v>259</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="B12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D12" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -1670,7 +1683,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
@@ -1678,8 +1691,8 @@
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
         <v>223</v>
       </c>
       <c r="B1" t="s">
@@ -1698,8 +1711,8 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1"/>
@@ -1711,7 +1724,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1730,8 +1743,8 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="47.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" ht="17.25">
+      <c r="A4" s="6" t="s">
         <v>240</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1745,7 +1758,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>226</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1762,8 +1775,8 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="30">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="6" t="s">
         <v>227</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1778,8 +1791,8 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="30">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1794,8 +1807,8 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="60">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:6" ht="30">
+      <c r="A8" s="6" t="s">
         <v>228</v>
       </c>
       <c r="B8" s="1"/>
@@ -1805,7 +1818,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="1"/>
@@ -1816,8 +1829,8 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="47.25">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:6" ht="17.25">
+      <c r="A10" s="6" t="s">
         <v>241</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1836,8 +1849,8 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="47.25">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:6" ht="17.25">
+      <c r="A11" s="6" t="s">
         <v>242</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1855,7 +1868,7 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1871,7 +1884,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1887,7 +1900,7 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1903,7 +1916,7 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1919,7 +1932,7 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="17.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>243</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1937,7 +1950,7 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1951,7 +1964,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>229</v>
       </c>
       <c r="B18" s="1"/>
@@ -1961,7 +1974,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>230</v>
       </c>
       <c r="B19" s="1"/>
@@ -1971,7 +1984,7 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1987,7 +2000,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2004,8 +2017,8 @@
         <v>225</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="32.25">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:6" ht="17.25">
+      <c r="A22" s="6" t="s">
         <v>244</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2023,7 +2036,7 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2038,8 +2051,8 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" ht="30">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:6">
+      <c r="A24" s="6" t="s">
         <v>77</v>
       </c>
       <c r="B24" s="1"/>
@@ -2051,7 +2064,7 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>83</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2069,7 +2082,7 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2086,8 +2099,8 @@
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" ht="30">
-      <c r="A27" s="7" t="s">
+    <row r="27" spans="1:6">
+      <c r="A27" s="6" t="s">
         <v>231</v>
       </c>
       <c r="B27" s="1"/>
@@ -2098,8 +2111,8 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" ht="30">
-      <c r="A28" s="7" t="s">
+    <row r="28" spans="1:6">
+      <c r="A28" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2115,7 +2128,7 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>91</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2130,8 +2143,8 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" ht="30">
-      <c r="A30" s="7" t="s">
+    <row r="30" spans="1:6">
+      <c r="A30" s="6" t="s">
         <v>95</v>
       </c>
       <c r="B30" s="1"/>
@@ -2145,7 +2158,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2163,7 +2176,7 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2183,7 +2196,7 @@
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>232</v>
       </c>
       <c r="B33" s="1"/>
@@ -2197,7 +2210,7 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>111</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2213,7 +2226,7 @@
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>121</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2228,8 +2241,8 @@
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" ht="30">
-      <c r="A36" s="7" t="s">
+    <row r="36" spans="1:6">
+      <c r="A36" s="6" t="s">
         <v>123</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2245,7 +2258,7 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>129</v>
       </c>
       <c r="B37" s="1"/>
@@ -2257,7 +2270,7 @@
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>131</v>
       </c>
       <c r="B38" s="1"/>
@@ -2271,7 +2284,7 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>135</v>
       </c>
       <c r="B39" s="1"/>
@@ -2282,8 +2295,8 @@
       </c>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" ht="30">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="1:6">
+      <c r="A40" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2299,7 +2312,7 @@
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>153</v>
       </c>
       <c r="B41" s="1"/>
@@ -2311,7 +2324,7 @@
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>155</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -2326,8 +2339,8 @@
       </c>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" ht="30">
-      <c r="A43" s="7" t="s">
+    <row r="43" spans="1:6">
+      <c r="A43" s="6" t="s">
         <v>233</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2344,8 +2357,8 @@
         <v>225</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30">
-      <c r="A44" s="7" t="s">
+    <row r="44" spans="1:6">
+      <c r="A44" s="6" t="s">
         <v>234</v>
       </c>
       <c r="B44" s="1"/>
@@ -2354,8 +2367,8 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" ht="30">
-      <c r="A45" s="7" t="s">
+    <row r="45" spans="1:6">
+      <c r="A45" s="6" t="s">
         <v>161</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -2371,7 +2384,7 @@
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>163</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2389,7 +2402,7 @@
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>165</v>
       </c>
       <c r="B47" s="1"/>
@@ -2400,8 +2413,8 @@
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" ht="30">
-      <c r="A48" s="7" t="s">
+    <row r="48" spans="1:6">
+      <c r="A48" s="6" t="s">
         <v>235</v>
       </c>
       <c r="B48" s="1"/>
@@ -2412,8 +2425,8 @@
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="1:6" ht="30">
-      <c r="A49" s="7" t="s">
+    <row r="49" spans="1:6">
+      <c r="A49" s="6" t="s">
         <v>236</v>
       </c>
       <c r="B49" s="1"/>
@@ -2429,7 +2442,7 @@
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>179</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2444,8 +2457,8 @@
       </c>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" ht="30">
-      <c r="A51" s="7" t="s">
+    <row r="51" spans="1:6">
+      <c r="A51" s="6" t="s">
         <v>181</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2460,8 +2473,8 @@
       </c>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:6" ht="32.25">
-      <c r="A52" s="7" t="s">
+    <row r="52" spans="1:6" ht="17.25">
+      <c r="A52" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2479,7 +2492,7 @@
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="6" t="s">
         <v>191</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2495,7 +2508,7 @@
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="6" t="s">
         <v>237</v>
       </c>
       <c r="B54" s="1"/>
@@ -2505,7 +2518,7 @@
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
         <v>197</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -2521,7 +2534,7 @@
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="6" t="s">
         <v>199</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2535,7 +2548,7 @@
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="6" t="s">
         <v>201</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -2553,7 +2566,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="6" t="s">
         <v>238</v>
       </c>
       <c r="B58" s="1"/>
@@ -2563,7 +2576,7 @@
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="6" t="s">
         <v>203</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -2578,8 +2591,8 @@
       </c>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:6" ht="30">
-      <c r="A60" s="7" t="s">
+    <row r="60" spans="1:6">
+      <c r="A60" s="6" t="s">
         <v>205</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -2595,7 +2608,7 @@
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="6" t="s">
         <v>207</v>
       </c>
       <c r="B61" s="1"/>
@@ -2606,8 +2619,8 @@
       </c>
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="1:6" ht="30">
-      <c r="A62" s="7" t="s">
+    <row r="62" spans="1:6">
+      <c r="A62" s="6" t="s">
         <v>211</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -2623,7 +2636,7 @@
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="6" t="s">
         <v>213</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -2638,8 +2651,8 @@
       </c>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="1:6" ht="30">
-      <c r="A64" s="7" t="s">
+    <row r="64" spans="1:6">
+      <c r="A64" s="6" t="s">
         <v>239</v>
       </c>
       <c r="B64" s="1"/>
@@ -2649,12 +2662,12 @@
       <c r="F64" s="1"/>
     </row>
     <row r="66" spans="1:1" ht="17.25">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="5" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="17.25">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="5" t="s">
         <v>247</v>
       </c>
     </row>
@@ -2677,19 +2690,19 @@
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2697,7 +2710,7 @@
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2705,7 +2718,7 @@
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2713,23 +2726,23 @@
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2737,15 +2750,15 @@
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2753,7 +2766,7 @@
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2761,15 +2774,15 @@
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2777,31 +2790,31 @@
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="30">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="45">
+    <row r="15" spans="1:2" ht="30">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="45">
+    <row r="16" spans="1:2" ht="30">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2809,7 +2822,7 @@
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2817,7 +2830,7 @@
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2825,7 +2838,7 @@
       <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2833,7 +2846,7 @@
       <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2841,7 +2854,7 @@
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2849,15 +2862,15 @@
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2865,7 +2878,7 @@
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2873,7 +2886,7 @@
       <c r="A25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2881,7 +2894,7 @@
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2889,7 +2902,7 @@
       <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2897,7 +2910,7 @@
       <c r="A28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2905,7 +2918,7 @@
       <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2913,7 +2926,7 @@
       <c r="A30" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2921,7 +2934,7 @@
       <c r="A31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2929,15 +2942,15 @@
       <c r="A32" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="30">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2945,7 +2958,7 @@
       <c r="A34" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2953,7 +2966,7 @@
       <c r="A35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2961,7 +2974,7 @@
       <c r="A36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2969,7 +2982,7 @@
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2977,15 +2990,15 @@
       <c r="A38" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="30">
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2993,7 +3006,7 @@
       <c r="A40" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3001,15 +3014,15 @@
       <c r="A41" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="30">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3017,7 +3030,7 @@
       <c r="A43" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3025,7 +3038,7 @@
       <c r="A44" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3033,7 +3046,7 @@
       <c r="A45" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3041,7 +3054,7 @@
       <c r="A46" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3049,7 +3062,7 @@
       <c r="A47" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3057,7 +3070,7 @@
       <c r="A48" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3065,7 +3078,7 @@
       <c r="A49" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3073,7 +3086,7 @@
       <c r="A50" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3081,7 +3094,7 @@
       <c r="A51" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3089,7 +3102,7 @@
       <c r="A52" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3097,7 +3110,7 @@
       <c r="A53" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3105,7 +3118,7 @@
       <c r="A54" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>120</v>
       </c>
     </row>
@@ -3113,31 +3126,31 @@
       <c r="A55" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="30">
+    <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="30">
+    <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="30">
+    <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3145,7 +3158,7 @@
       <c r="A59" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3153,15 +3166,15 @@
       <c r="A60" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="30">
+    <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3169,7 +3182,7 @@
       <c r="A62" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3177,7 +3190,7 @@
       <c r="A63" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3185,23 +3198,23 @@
       <c r="A64" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="30">
+    <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="60">
+    <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>144</v>
       </c>
     </row>
@@ -3209,23 +3222,23 @@
       <c r="A67" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="30">
+    <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="45">
+    <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="3" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3233,7 +3246,7 @@
       <c r="A70" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="3" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3241,7 +3254,7 @@
       <c r="A71" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="3" t="s">
         <v>154</v>
       </c>
     </row>
@@ -3249,15 +3262,15 @@
       <c r="A72" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="60">
+    <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3265,15 +3278,15 @@
       <c r="A74" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="30">
+    <row r="75" spans="1:2">
       <c r="A75" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="3" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3281,7 +3294,7 @@
       <c r="A76" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="3" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3289,15 +3302,15 @@
       <c r="A77" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="30">
+    <row r="78" spans="1:2">
       <c r="A78" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="3" t="s">
         <v>168</v>
       </c>
     </row>
@@ -3305,7 +3318,7 @@
       <c r="A79" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3313,7 +3326,7 @@
       <c r="A80" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="3" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3321,7 +3334,7 @@
       <c r="A81" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="3" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3329,15 +3342,15 @@
       <c r="A82" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="45">
+    <row r="83" spans="1:2">
       <c r="A83" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="3" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3345,15 +3358,15 @@
       <c r="A84" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="30">
+    <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="3" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3361,7 +3374,7 @@
       <c r="A86" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="3" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3369,15 +3382,15 @@
       <c r="A87" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="30">
+    <row r="88" spans="1:2">
       <c r="A88" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="3" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3385,7 +3398,7 @@
       <c r="A89" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="3" t="s">
         <v>190</v>
       </c>
     </row>
@@ -3393,15 +3406,15 @@
       <c r="A90" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="30">
+    <row r="91" spans="1:2">
       <c r="A91" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="3" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3409,7 +3422,7 @@
       <c r="A92" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="3" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3417,7 +3430,7 @@
       <c r="A93" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="3" t="s">
         <v>198</v>
       </c>
     </row>
@@ -3425,7 +3438,7 @@
       <c r="A94" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="3" t="s">
         <v>200</v>
       </c>
     </row>
@@ -3433,7 +3446,7 @@
       <c r="A95" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="3" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3441,15 +3454,15 @@
       <c r="A96" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="30">
+    <row r="97" spans="1:2">
       <c r="A97" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="3" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3457,7 +3470,7 @@
       <c r="A98" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="3" t="s">
         <v>208</v>
       </c>
     </row>
@@ -3465,15 +3478,15 @@
       <c r="A99" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="30">
+    <row r="100" spans="1:2">
       <c r="A100" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="3" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3481,7 +3494,7 @@
       <c r="A101" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="3" t="s">
         <v>214</v>
       </c>
     </row>
@@ -3489,7 +3502,7 @@
       <c r="A102" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="3" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3497,7 +3510,7 @@
       <c r="A103" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="3" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3505,7 +3518,7 @@
       <c r="A104" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="3" t="s">
         <v>220</v>
       </c>
     </row>
@@ -3513,7 +3526,7 @@
       <c r="A105" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B105" s="3" t="s">
         <v>222</v>
       </c>
     </row>

</xml_diff>